<commit_message>
fix giao dien blog
</commit_message>
<xml_diff>
--- a/MVC/Views/pages/admin/quanlyBlog/BlogExcel.xlsx
+++ b/MVC/Views/pages/admin/quanlyBlog/BlogExcel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>ID Blog</t>
   </si>
@@ -35,82 +35,40 @@
     <t>Hình Ảnh</t>
   </si>
   <si>
-    <t>duy</t>
-  </si>
-  <si>
-    <t>đẹp</t>
-  </si>
-  <si>
-    <t>2022-11-08</t>
-  </si>
-  <si>
-    <t>khánh</t>
-  </si>
-  <si>
-    <t>quá đẹp</t>
-  </si>
-  <si>
-    <t>2022-10-31</t>
-  </si>
-  <si>
-    <t>cao</t>
-  </si>
-  <si>
-    <t>đẹp ghê</t>
-  </si>
-  <si>
-    <t>2022-10-19</t>
-  </si>
-  <si>
-    <t>phượng</t>
-  </si>
-  <si>
-    <t>đẹp nhờ</t>
-  </si>
-  <si>
-    <t>2022-10-12</t>
-  </si>
-  <si>
-    <t>ngân xinh gái</t>
-  </si>
-  <si>
-    <t>đẹp rùi</t>
-  </si>
-  <si>
-    <t>2022-11-22</t>
-  </si>
-  <si>
-    <t>quang đập trai</t>
-  </si>
-  <si>
-    <t>dkjf</t>
-  </si>
-  <si>
-    <t>4b8aa02f3224982dd9acf84ad6529a39.jpg</t>
-  </si>
-  <si>
-    <t>hi</t>
-  </si>
-  <si>
-    <t>skkd</t>
+    <t>Bóng đá</t>
+  </si>
+  <si>
+    <t>NÔI DUNG BLOG</t>
   </si>
   <si>
     <t>2022-12-08</t>
   </si>
   <si>
-    <t>1-152753_928.jpg</t>
-  </si>
-  <si>
-    <t>kh</t>
-  </si>
-  <si>
-    <t>kđs</t>
-  </si>
-  <si>
-    <t>2022-12-07</t>
-  </si>
-  <si>
-    <t>121994622_1236523253371713_609227557238820667_n.jpg</t>
+    <t>75258550_2545915118988163_3298790051630022656_n.png</t>
+  </si>
+  <si>
+    <t>Bóng Chuyền</t>
+  </si>
+  <si>
+    <t>311038288_555308266596129_7246856222758665646_n.jpeg</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>20*7.png</t>
+  </si>
+  <si>
+    <t>Cầu Long</t>
+  </si>
+  <si>
+    <t>Nội dung</t>
+  </si>
+  <si>
+    <t>Screenshot 2022-10-31 at 15.44.44.png</t>
+  </si>
+  <si>
+    <t>Dương Tùng.png</t>
   </si>
 </sst>
 </file>
@@ -475,20 +433,20 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="17.567139" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="10.568848" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="16.424561" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="61.270752" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="62.41333" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -513,7 +471,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -522,143 +480,91 @@
         <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2">
-        <v>23</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2">
-        <v>56</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2">
-        <v>23</v>
-      </c>
-      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="2">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>31</v>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>